<commit_message>
Casos de prueba sprint 3
</commit_message>
<xml_diff>
--- a/docs/testing_final/CasosDePrueba.xlsx
+++ b/docs/testing_final/CasosDePrueba.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\DMH\DigitalMoneyHouse\docs\testing_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0434A2D3-86DC-429D-8DAF-C091BE2D10C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CB529A-1F78-47B4-AC49-647EFF3426C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{0C2BC477-9FEC-4983-8494-E703DAC6212C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{0C2BC477-9FEC-4983-8494-E703DAC6212C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="124">
   <si>
     <t>ID</t>
   </si>
@@ -311,13 +312,129 @@
   </si>
   <si>
     <t>Cuenta existente, token válido, tarjeta asociada</t>
+  </si>
+  <si>
+    <t>TC-ACT-01</t>
+  </si>
+  <si>
+    <t>GET /accounts/{accountId}/activity</t>
+  </si>
+  <si>
+    <t>Obtener listado de actividades</t>
+  </si>
+  <si>
+    <t>200 OK + lista de actividades</t>
+  </si>
+  <si>
+    <t>TC-ACT-02</t>
+  </si>
+  <si>
+    <t>GET /accounts/{accountId}/activity/{transferId}</t>
+  </si>
+  <si>
+    <t>Obtener detalle de una actividad</t>
+  </si>
+  <si>
+    <t>200 OK + actividad solicitada</t>
+  </si>
+  <si>
+    <t>POST /accounts/{accountId}/transferences</t>
+  </si>
+  <si>
+    <t>Ingresar dinero a la cuenta</t>
+  </si>
+  <si>
+    <t>Cuenta existente, token válido, request body con datos válidos</t>
+  </si>
+  <si>
+    <t>201 Created + transferencia/actividad</t>
+  </si>
+  <si>
+    <t>TC-ACT-03</t>
+  </si>
+  <si>
+    <t>Obtener listado de actividades sin token</t>
+  </si>
+  <si>
+    <t>Request sin token o token inválido</t>
+  </si>
+  <si>
+    <t>Obtener listado de actividades de cuenta</t>
+  </si>
+  <si>
+    <t>que no pertenece al usuario</t>
+  </si>
+  <si>
+    <t>usuario o inexistente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>403 Forbidden o 404 Not Found</t>
+  </si>
+  <si>
+    <t>TC-DET-02</t>
+  </si>
+  <si>
+    <t>TC-DET-01</t>
+  </si>
+  <si>
+    <t>Obtener detalle de una actividad con transferId inexistente</t>
+  </si>
+  <si>
+    <t>TC-DET-03</t>
+  </si>
+  <si>
+    <t>Obtener detalle de una actividad de una cuenta ajena</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">La cuenta </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>{accountId}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pertenece a otro usuario</t>
+    </r>
+  </si>
+  <si>
+    <t>Cuenta existente, token válido, {transferId} inexistente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuenta existente, token valido, {accountId} no perteneciente al </t>
+  </si>
+  <si>
+    <t xml:space="preserve">403 Forbidden </t>
+  </si>
+  <si>
+    <t>Registrar ingreso con monto cero o negativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuenta existente, token válido, {accountId} existente y </t>
+  </si>
+  <si>
+    <t>pertenece al usuario y monto &lt;= 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +455,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -381,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -391,6 +513,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,10 +831,10 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11.21875" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
@@ -720,7 +843,7 @@
     <col min="5" max="5" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -740,7 +863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -760,7 +883,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -780,7 +903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -800,7 +923,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -820,7 +943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -840,7 +963,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -860,7 +983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -889,11 +1012,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CF5D3C-D30A-4AA9-8158-7A2C0F3CE0B5}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.88671875" customWidth="1"/>
     <col min="2" max="2" width="38.77734375" customWidth="1"/>
@@ -902,7 +1025,7 @@
     <col min="5" max="5" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -925,7 +1048,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -948,7 +1071,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -971,7 +1094,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -994,7 +1117,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1017,7 +1140,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1040,7 +1163,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>57</v>
       </c>
@@ -1063,7 +1186,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>61</v>
       </c>
@@ -1086,7 +1209,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>67</v>
       </c>
@@ -1109,7 +1232,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1132,7 +1255,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>78</v>
       </c>
@@ -1155,7 +1278,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>82</v>
       </c>
@@ -1178,7 +1301,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>85</v>
       </c>
@@ -1201,7 +1324,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
         <v>88</v>
       </c>
@@ -1222,6 +1345,253 @@
       </c>
       <c r="G14" s="3" t="s">
         <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C6572B-C6C5-4492-A5CC-AADEF23AEF1E}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="40.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49" customWidth="1"/>
+    <col min="4" max="4" width="52.21875" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="D11" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrego dockerfile y docker compose
</commit_message>
<xml_diff>
--- a/docs/testing_final/CasosDePrueba.xlsx
+++ b/docs/testing_final/CasosDePrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\DMH\DigitalMoneyHouse\docs\testing_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CB529A-1F78-47B4-AC49-647EFF3426C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8666EB-D259-43A6-BE7D-C1DFB860EA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{0C2BC477-9FEC-4983-8494-E703DAC6212C}"/>
   </bookViews>
@@ -338,9 +338,6 @@
     <t>200 OK + actividad solicitada</t>
   </si>
   <si>
-    <t>POST /accounts/{accountId}/transferences</t>
-  </si>
-  <si>
     <t>Ingresar dinero a la cuenta</t>
   </si>
   <si>
@@ -428,6 +425,9 @@
   </si>
   <si>
     <t>pertenece al usuario y monto &lt;= 0</t>
+  </si>
+  <si>
+    <t>POST /accounts/{accountId}/transactions/deposit</t>
   </si>
 </sst>
 </file>
@@ -1359,12 +1359,12 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="40.5546875" customWidth="1"/>
+    <col min="2" max="2" width="42.21875" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
     <col min="4" max="4" width="52.21875" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
         <v>97</v>
@@ -1445,16 +1445,16 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
         <v>100</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" t="s">
         <v>102</v>
-      </c>
-      <c r="E4" t="s">
-        <v>103</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -1471,10 +1471,10 @@
         <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>76</v>
@@ -1488,19 +1488,19 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>11</v>
@@ -1511,27 +1511,27 @@
     </row>
     <row r="7" spans="1:7">
       <c r="C7" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>84</v>
@@ -1545,19 +1545,19 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" t="s">
         <v>116</v>
       </c>
-      <c r="D9" t="s">
-        <v>117</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>11</v>
@@ -1571,13 +1571,13 @@
         <v>78</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" t="s">
         <v>121</v>
-      </c>
-      <c r="D10" t="s">
-        <v>122</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>15</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="D11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>